<commit_message>
Added table with parameters used in simulations
</commit_message>
<xml_diff>
--- a/SEC_Tables.xlsx
+++ b/SEC_Tables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HCN-by-Alleles" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>CYP79D15</t>
   </si>
@@ -42,6 +43,108 @@
   </si>
   <si>
     <t>Decrease</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Maximum migration rate (m)</t>
+  </si>
+  <si>
+    <t>Maximum carrying capacity (Kmax)</t>
+  </si>
+  <si>
+    <t>Minimum carrying capacity (Kmin)</t>
+  </si>
+  <si>
+    <t>Number of rows</t>
+  </si>
+  <si>
+    <t>Number of columns</t>
+  </si>
+  <si>
+    <t>Founder proportion</t>
+  </si>
+  <si>
+    <t>Maximum population creation probability</t>
+  </si>
+  <si>
+    <t>Maximum selection coefficient (smax)</t>
+  </si>
+  <si>
+    <t>Frequency of dominant CYP79D15 (pA)</t>
+  </si>
+  <si>
+    <t>Frequency of dominant Li (pB)</t>
+  </si>
+  <si>
+    <t>Number of generations</t>
+  </si>
+  <si>
+    <t>Number of simulations</t>
+  </si>
+  <si>
+    <t>Determines the maximum proportion of alleles (CYP79D15 and Li) exchanged between any two populations. The actual proportion depends on the distance between populations (Equation X)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determines the carrying capacity of the largest habitat patch on the landscape. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determines the carrying capacity of the smallest habitat patch on the landscape. </t>
+  </si>
+  <si>
+    <t>Intrinsic rate of population increase</t>
+  </si>
+  <si>
+    <t>Number of rows on the landscape. Fixed at 1 since we are simulating a one-dimensional, linear matrix.</t>
+  </si>
+  <si>
+    <t>Number of columns on the landscape. Fixed at 40 since we are simulating 40 linearly distributed patches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion of alleles sampled when founding a new populations. Lower proportions results in stronger effects of drift. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum probability that a new population is created. Actual probability depends on the populations size such that larger populations have a greater probability of creating new ones. Values is fixed at 1.0 so that populations at carrying capacity are guarenteed to found new populations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum strength of selection acting on cyanogenic or acyanogenic genotypes. Actual strength of selection depends on position in the landscape matrix. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial frequency of the dominant allele at the CYP79D15 locus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial frequency of the dominant allele at the Li locus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intrinsic growth rate parameter used in logistic equation of population growth. Fixed at 1.5. </t>
+  </si>
+  <si>
+    <t>Number of simulation to run. Fixed at 1000.</t>
+  </si>
+  <si>
+    <t>Number of generations to run simulations once all patched on the landscape have been colonized with populations. Fixed at 500</t>
+  </si>
+  <si>
+    <t>Mechanism controlled</t>
+  </si>
+  <si>
+    <t>Gene flow</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Within-population dynamics</t>
+  </si>
+  <si>
+    <t>Drift (Case 2, see text)</t>
+  </si>
+  <si>
+    <t>Drift (Case 1, see text)</t>
   </si>
 </sst>
 </file>
@@ -213,7 +316,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -251,6 +354,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -265,91 +383,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="double">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="double">
-          <color auto="1"/>
-        </top>
-        <bottom style="double">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="double">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -401,10 +434,95 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="double">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -418,7 +536,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -426,8 +544,8 @@
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" name="CYP79D15" dataDxfId="2"/>
-    <tableColumn id="2" name="Li" dataDxfId="5"/>
-    <tableColumn id="3" name="HCN" dataDxfId="4"/>
+    <tableColumn id="2" name="Li" dataDxfId="1"/>
+    <tableColumn id="3" name="HCN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -698,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
@@ -768,4 +886,164 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>